<commit_message>
SBML reports generated for SBML validation
</commit_message>
<xml_diff>
--- a/sbml/annotations/Hepatic_Glucose_Model_Annotations.xlsx
+++ b/sbml/annotations/Hepatic_Glucose_Model_Annotations.xlsx
@@ -85,7 +85,7 @@
     <t>3.6.1.1</t>
   </si>
   <si>
-    <t>NTKGTP</t>
+    <t>NDKGTP</t>
   </si>
   <si>
     <t>2.7.4.6</t>
@@ -971,9 +971,9 @@
   <dimension ref="A1:F157"/>
   <sheetViews>
     <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="true" topLeftCell="A1" view="normal" windowProtection="true" workbookViewId="0" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100">
-      <pane activePane="bottomLeft" state="frozen" topLeftCell="A89" xSplit="0" ySplit="1"/>
+      <pane activePane="bottomLeft" state="frozen" topLeftCell="A2" xSplit="0" ySplit="1"/>
       <selection activeCell="A1" activeCellId="0" pane="topLeft" sqref="A1"/>
-      <selection activeCell="B157" activeCellId="0" pane="bottomLeft" sqref="B157"/>
+      <selection activeCell="A8" activeCellId="0" pane="bottomLeft" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.1"/>
@@ -4047,7 +4047,7 @@
         <v>180</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.9" outlineLevel="0" r="157">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="157">
       <c r="A157" s="1" t="s">
         <v>177</v>
       </c>
@@ -4086,7 +4086,7 @@
   <dimension ref="A1:E14"/>
   <sheetViews>
     <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="false" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100">
-      <selection activeCell="H25" activeCellId="1" pane="topLeft" sqref="B157 H25"/>
+      <selection activeCell="H25" activeCellId="0" pane="topLeft" sqref="H25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -4272,7 +4272,7 @@
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="false" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100">
-      <selection activeCell="A1" activeCellId="1" pane="topLeft" sqref="B157 A1"/>
+      <selection activeCell="A1" activeCellId="0" pane="topLeft" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>

</xml_diff>